<commit_message>
Stařec a moře a O myších a lidech
</commit_message>
<xml_diff>
--- a/tabulkaNaVyberKnih.xlsx
+++ b/tabulkaNaVyberKnih.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Maturitka\seanceZapisy\excelTabulkaLiteraturyNaMaturitu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\6. Maturitka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2B565B-8998-41F1-820A-E6049A00C712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212EBF12-D9B4-43AD-AAC6-CECC57CAABAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{94871187-8663-4E32-9055-774820EF964F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94871187-8663-4E32-9055-774820EF964F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -952,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B08A221A-4539-429B-94E8-A725B3A71C58}">
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="K19">
         <f>SUMIF($G$3:$G$73, "Ano", $D$3:$D$73)</f>
-        <v>1748</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1434,9 +1434,6 @@
       </c>
       <c r="E25" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="G25" t="s">
-        <v>142</v>
       </c>
       <c r="J25" t="s">
         <v>130</v>
@@ -1958,6 +1955,9 @@
       </c>
       <c r="E55" s="4" t="s">
         <v>129</v>
+      </c>
+      <c r="G55" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2385,7 +2385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED5601A-EFF2-4866-801D-2AC2276BEE6F}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -2488,10 +2488,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="str">
-        <v>J. Neruda</v>
+        <v>E. Hemingway</v>
       </c>
       <c r="C9" s="2" t="str">
-        <v>Malostranské povídky</v>
+        <v>Stařec a moře</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2499,10 +2499,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="str">
-        <v>E. Hemingway</v>
+        <v>J. Steinbeck</v>
       </c>
       <c r="C10" s="2" t="str">
-        <v>Stařec a moře</v>
+        <v>O myších a lidech</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2510,10 +2510,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="str">
-        <v>J. Steinbeck</v>
+        <v>R. Rolland</v>
       </c>
       <c r="C11" s="2" t="str">
-        <v>O myších a lidech</v>
+        <v>Petr a Lucie</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2521,10 +2521,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="str">
-        <v>R. Rolland</v>
+        <v>G. Orwell</v>
       </c>
       <c r="C12" s="2" t="str">
-        <v>Petr a Lucie</v>
+        <v>Farma zvířat</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2534,8 +2534,8 @@
       <c r="B13" s="2" t="str">
         <v>G. Orwell</v>
       </c>
-      <c r="C13" s="2" t="str">
-        <v>Farma zvířat</v>
+      <c r="C13" s="2">
+        <v>1984</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2543,10 +2543,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="str">
-        <v>G. Orwell</v>
-      </c>
-      <c r="C14" s="2">
-        <v>1984</v>
+        <v>V. Dyk</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <v>Krysař</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,10 +2554,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="str">
-        <v>V. Dyk</v>
+        <v>J. Wolker</v>
       </c>
       <c r="C15" s="2" t="str">
-        <v>Krysař</v>
+        <v>Balada o námořníkovi</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,10 +2565,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="str">
-        <v>J. Wolker</v>
+        <v>L. Fuks</v>
       </c>
       <c r="C16" s="2" t="str">
-        <v>Balada o námořníkovi</v>
+        <v>Spalovač mrtvol</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,10 +2576,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="str">
-        <v>L. Fuks</v>
+        <v>M. Kundera</v>
       </c>
       <c r="C17" s="2" t="str">
-        <v>Spalovač mrtvol</v>
+        <v>Falešný autostop</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>